<commit_message>
TR: Lộc - Sắp xếp nhật ký giao dịch tài chính
</commit_message>
<xml_diff>
--- a/UsedPrompts.xlsx
+++ b/UsedPrompts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\RaNgoaiLamChu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A09C26-03FF-48E9-8292-768EC7831740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4D4F7-C433-4A13-94A1-AA1EF36E0258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1596" windowWidth="15900" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="1596" windowWidth="15900" windowHeight="10020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11-17 tháng 3" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Lộc</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>TR8</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Lộc: 77, Khải: 5</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +207,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -297,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -330,6 +342,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA287BCE-33B2-4487-BC5A-2D0267491B91}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -893,18 +908,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603100F5-DB9A-4E78-B229-8D3855C72AFE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
@@ -920,8 +936,11 @@
       <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -941,8 +960,11 @@
         <f t="array" aca="1" ref="E2" ca="1">SUM(IF(LEFT(INDIRECT("'"&amp;A2&amp;"'!D:D"),2)="TR",5,IF(LEFT(INDIRECT("'"&amp;A2&amp;"'!D:D"),2)="CR",5,IF(LEFT(INDIRECT("'"&amp;A2&amp;"'!D:D"),2)="CG",4,IF(LEFT(INDIRECT("'"&amp;A2&amp;"'!D:D"),2)="PR",4,0)))))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -963,21 +985,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>

</xml_diff>